<commit_message>
Bond curve first working files
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_010_ITALY.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_010_ITALY.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="19065" yWindow="-15" windowWidth="19110" windowHeight="12045" tabRatio="684" activeTab="5"/>
+    <workbookView xWindow="19065" yWindow="-15" windowWidth="19110" windowHeight="12045" tabRatio="684"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="13" r:id="rId1"/>
@@ -158,12 +158,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="178" formatCode="0.0000%"/>
-    <numFmt numFmtId="180" formatCode="0.0000"/>
-    <numFmt numFmtId="181" formatCode="General_)"/>
-    <numFmt numFmtId="182" formatCode="#,##0.0;#,##0.0"/>
-    <numFmt numFmtId="183" formatCode="ddd\,\ d\-mmm\-yyyy\,\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="General_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0;#,##0.0"/>
+    <numFmt numFmtId="169" formatCode="ddd\,\ d\-mmm\-yyyy\,\ hh:mm:ss"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -173,6 +173,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -473,12 +474,12 @@
     <xf numFmtId="38" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="182" fontId="5" fillId="2" borderId="0">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -490,23 +491,23 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="183" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,8 +948,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -1172,13 +1173,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_CCTs.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(D3:D20),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0003605380_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -1462,9 +1463,9 @@
         <f>IF(ISNA(C17),NA(),_xll.qlSimpleQuote(C17,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E17" s="33" t="str">
+      <c r="E17" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D17)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F17" s="23"/>
     </row>
@@ -1481,9 +1482,9 @@
         <f>IF(ISNA(C18),NA(),_xll.qlSimpleQuote(C18,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E18" s="33" t="str">
+      <c r="E18" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D18)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F18" s="23"/>
     </row>
@@ -1500,9 +1501,9 @@
         <f>IF(ISNA(C19),NA(),_xll.qlSimpleQuote(C19,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E19" s="33" t="str">
+      <c r="E19" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D19)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F19" s="23"/>
     </row>
@@ -1519,9 +1520,9 @@
         <f>IF(ISNA(C20),NA(),_xll.qlSimpleQuote(C20,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E20" s="33" t="str">
+      <c r="E20" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D20)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F20" s="23"/>
     </row>
@@ -1581,13 +1582,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPs.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(D3:D102),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0003799597_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -3428,13 +3429,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPInflation.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(D3:D12,SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0004216351_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -3678,13 +3679,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPCouponsFebAug.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(D3:D64),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0003106561_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -4831,7 +4832,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4866,13 +4867,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPCouponsMayNov.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(D3:D47),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0001247052_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -5701,9 +5702,9 @@
         <f>IF(ISNA(B46),NA(),_xll.qlSimpleQuote(C46,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E46" s="33" t="str">
+      <c r="E46" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D46)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F46" s="23"/>
     </row>
@@ -5720,9 +5721,9 @@
         <f>IF(ISNA(B47),NA(),_xll.qlSimpleQuote(C47,,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E47" s="33" t="str">
+      <c r="E47" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D47)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F47" s="23"/>
     </row>
@@ -5782,13 +5783,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPResiduesFebAug.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(C3:D24),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0003106389_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -6180,9 +6181,9 @@
         <f>IF(ISNA(B23),NA(),_xll.qlSimpleQuote($B23&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E23" s="33" t="str">
+      <c r="E23" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C23)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F23" s="23"/>
     </row>
@@ -6199,9 +6200,9 @@
         <f>IF(ISNA(B24),NA(),_xll.qlSimpleQuote($B24&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E24" s="33" t="str">
+      <c r="E24" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C24)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F24" s="23"/>
     </row>
@@ -6261,13 +6262,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_BTPResiduesMayNov.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(C3:D10),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'IT0001461844_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -6393,9 +6394,9 @@
         <f>IF(ISNA(B9),NA(),_xll.qlSimpleQuote($B9&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E9" s="33" t="str">
+      <c r="E9" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C9)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F9" s="23"/>
     </row>
@@ -6412,9 +6413,9 @@
         <f>IF(ISNA(B10),NA(),_xll.qlSimpleQuote($B10&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E10" s="33" t="str">
+      <c r="E10" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C10)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F10" s="23"/>
     </row>
@@ -6474,13 +6475,13 @@
         <f>Currency&amp;"_"&amp;C1&amp;".xml"</f>
         <v>EUR_010_CCTResidues.xml</v>
       </c>
-      <c r="D2" s="22" t="e">
+      <c r="D2" s="22" t="str">
         <f>IF(Serialize,_xll.ohObjectSave(_xll.ohPack(C3:D9),SerializationPath&amp;C2,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="31" t="str">
+        <v>---</v>
+      </c>
+      <c r="E2" s="31" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(D2)</f>
-        <v>ohObjectSave - ObjectHandler error: attempt to retrieve object with unknown ID 'CCT EU 2015-12 RESIDUE_Quote'</v>
+        <v>#NAME?</v>
       </c>
       <c r="F2" s="23"/>
     </row>
@@ -6555,9 +6556,9 @@
         <f>IF(ISNA(B6),NA(),_xll.qlSimpleQuote($B6&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="33" t="str">
+      <c r="E6" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C6)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F6" s="23"/>
     </row>
@@ -6575,9 +6576,9 @@
         <f>IF(ISNA(B7),NA(),_xll.qlSimpleQuote($B7&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E7" s="33" t="str">
+      <c r="E7" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C7)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F7" s="23"/>
     </row>
@@ -6595,9 +6596,9 @@
         <f>IF(ISNA(B8),NA(),_xll.qlSimpleQuote($B8&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E8" s="33" t="str">
+      <c r="E8" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C8)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F8" s="23"/>
     </row>
@@ -6615,9 +6616,9 @@
         <f>IF(ISNA(B9),NA(),_xll.qlSimpleQuote($B9&amp;"ResPrem"&amp;QuoteSuffix,0,PriceTickValue,Permanent,Trigger,ObjectOverwrite))</f>
         <v>#N/A</v>
       </c>
-      <c r="E9" s="33" t="str">
+      <c r="E9" s="33" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(C9)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="F9" s="23"/>
     </row>

</xml_diff>